<commit_message>
Added: display grade and review button correspond to finalized status
</commit_message>
<xml_diff>
--- a/backend/uploads/Template-import-student (2).xlsx
+++ b/backend/uploads/Template-import-student (2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SonNguyen\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32C8A1F-453B-496E-B94F-790A5AA06C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E349328-AF8E-4EA5-B1E6-A413CF74D9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{F8A6FD58-EA86-4CE5-A8B3-FC50B2269177}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>dat</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>MSSV</t>
   </si>
@@ -45,13 +42,7 @@
     <t>Ten</t>
   </si>
   <si>
-    <t>son</t>
-  </si>
-  <si>
-    <t>quang</t>
-  </si>
-  <si>
-    <t>admin</t>
+    <t>sol student 1</t>
   </si>
 </sst>
 </file>
@@ -403,52 +394,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE7D42B7-2D73-4F88-9C0D-096B273C4B4C}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>18313</v>
+        <v>1815371</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>18537</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>18230</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>18000</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>